<commit_message>
appendix B and updates in paper
</commit_message>
<xml_diff>
--- a/Tables/mechanism.xlsx
+++ b/Tables/mechanism.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xps-seira\Dropbox\Apps\ShareLaTeX\Donde2019\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xps-seira\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA42F946-952E-4FAB-9886-269ECFF9206C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C34203-37F8-4C29-B7A7-8BF04BE01DA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13872" yWindow="-13068" windowWidth="23256" windowHeight="13176" xr2:uid="{97C891ED-ED1B-44F0-A8FF-ED720B6E75ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{97C891ED-ED1B-44F0-A8FF-ED720B6E75ED}"/>
   </bookViews>
   <sheets>
     <sheet name="mechanism" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>Observations</t>
   </si>
@@ -46,9 +48,6 @@
   </si>
   <si>
     <t>Size of pay.</t>
-  </si>
-  <si>
-    <t>Trans. cost</t>
   </si>
   <si>
     <t>Days to rec.</t>
@@ -195,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,6 +215,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -262,9 +267,6 @@
           <cell r="D2" t="str">
             <v>(3)</v>
           </cell>
-          <cell r="E2" t="str">
-            <v>(4)</v>
-          </cell>
           <cell r="F2" t="str">
             <v>(5)</v>
           </cell>
@@ -274,31 +276,25 @@
           <cell r="H2" t="str">
             <v>(7)</v>
           </cell>
-          <cell r="I2" t="str">
-            <v>(8)</v>
-          </cell>
         </row>
         <row r="5">
           <cell r="B5" t="str">
-            <v>-8.54***</v>
+            <v>-8.54</v>
           </cell>
           <cell r="C5" t="str">
-            <v>0.19***</v>
+            <v>0.19</v>
           </cell>
           <cell r="D5" t="str">
-            <v>37.7</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>15.5***</v>
+            <v>34.0</v>
           </cell>
           <cell r="F5" t="str">
-            <v>-8.51***</v>
+            <v>-8.52</v>
           </cell>
           <cell r="G5" t="str">
             <v>-0.0068</v>
           </cell>
           <cell r="H5" t="str">
-            <v>0.081***</v>
+            <v>0.081</v>
           </cell>
         </row>
         <row r="6">
@@ -309,10 +305,7 @@
             <v>(0.044)</v>
           </cell>
           <cell r="D6" t="str">
-            <v>(51.0)</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>(4.57)</v>
+            <v>(51.2)</v>
           </cell>
           <cell r="F6" t="str">
             <v>(2.68)</v>
@@ -344,9 +337,6 @@
           <cell r="D83" t="str">
             <v/>
           </cell>
-          <cell r="E83" t="str">
-            <v/>
-          </cell>
           <cell r="F83" t="str">
             <v/>
           </cell>
@@ -357,7 +347,7 @@
             <v/>
           </cell>
           <cell r="I83" t="str">
-            <v>0.88***</v>
+            <v>0.88</v>
           </cell>
         </row>
         <row r="84">
@@ -371,9 +361,6 @@
             <v/>
           </cell>
           <cell r="D84" t="str">
-            <v/>
-          </cell>
-          <cell r="E84" t="str">
             <v/>
           </cell>
           <cell r="F84" t="str">
@@ -409,9 +396,6 @@
           <cell r="D101" t="str">
             <v>5085</v>
           </cell>
-          <cell r="E101" t="str">
-            <v>2719</v>
-          </cell>
           <cell r="F101" t="str">
             <v>2490</v>
           </cell>
@@ -436,10 +420,7 @@
             <v>1.18</v>
           </cell>
           <cell r="D103" t="str">
-            <v>829.7</v>
-          </cell>
-          <cell r="E103" t="str">
-            <v>81.7</v>
+            <v>830.5</v>
           </cell>
           <cell r="F103" t="str">
             <v>92.7</v>
@@ -470,19 +451,16 @@
       <sheetData sheetId="0">
         <row r="5">
           <cell r="B5" t="str">
-            <v>-3.01***</v>
+            <v>-2.97</v>
           </cell>
           <cell r="C5" t="str">
-            <v>0.17***</v>
+            <v>0.17</v>
           </cell>
           <cell r="D5" t="str">
-            <v>-68.8</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>20.1***</v>
+            <v>-72.6</v>
           </cell>
           <cell r="F5" t="str">
-            <v>-1.59</v>
+            <v>-1.45</v>
           </cell>
           <cell r="G5" t="str">
             <v>-0.021</v>
@@ -499,13 +477,10 @@
             <v>(0.051)</v>
           </cell>
           <cell r="D6" t="str">
-            <v>(46.6)</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>(5.51)</v>
+            <v>(46.5)</v>
           </cell>
           <cell r="F6" t="str">
-            <v>(3.22)</v>
+            <v>(3.21)</v>
           </cell>
           <cell r="G6" t="str">
             <v>(0.020)</v>
@@ -534,9 +509,6 @@
           <cell r="D83" t="str">
             <v/>
           </cell>
-          <cell r="E83" t="str">
-            <v/>
-          </cell>
           <cell r="F83" t="str">
             <v/>
           </cell>
@@ -547,7 +519,7 @@
             <v/>
           </cell>
           <cell r="I83" t="str">
-            <v>0.88***</v>
+            <v>0.88</v>
           </cell>
         </row>
         <row r="84">
@@ -563,9 +535,6 @@
           <cell r="D84" t="str">
             <v/>
           </cell>
-          <cell r="E84" t="str">
-            <v/>
-          </cell>
           <cell r="F84" t="str">
             <v/>
           </cell>
@@ -581,7 +550,7 @@
         </row>
         <row r="95">
           <cell r="I95" t="str">
-            <v>0.0063</v>
+            <v>0.0060</v>
           </cell>
         </row>
         <row r="96">
@@ -591,28 +560,25 @@
         </row>
         <row r="101">
           <cell r="B101" t="str">
-            <v>4656</v>
+            <v>4655</v>
           </cell>
           <cell r="C101" t="str">
-            <v>4758</v>
+            <v>4757</v>
           </cell>
           <cell r="D101" t="str">
-            <v>4758</v>
-          </cell>
-          <cell r="E101" t="str">
-            <v>2409</v>
+            <v>4757</v>
           </cell>
           <cell r="F101" t="str">
-            <v>2075</v>
+            <v>2073</v>
           </cell>
           <cell r="G101" t="str">
-            <v>4758</v>
+            <v>4757</v>
           </cell>
           <cell r="H101" t="str">
-            <v>4734</v>
+            <v>4733</v>
           </cell>
           <cell r="I101" t="str">
-            <v>4734</v>
+            <v>4733</v>
           </cell>
         </row>
       </sheetData>
@@ -631,25 +597,22 @@
       <sheetData sheetId="0">
         <row r="5">
           <cell r="B5" t="str">
-            <v>-2.38**</v>
+            <v>-2.40</v>
           </cell>
           <cell r="C5" t="str">
-            <v>0.13***</v>
+            <v>0.13</v>
           </cell>
           <cell r="D5" t="str">
-            <v>-54.2</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>16.5***</v>
+            <v>-53.7</v>
           </cell>
           <cell r="F5" t="str">
-            <v>1.02</v>
+            <v>0.98</v>
           </cell>
           <cell r="G5" t="str">
             <v>-0.0077</v>
           </cell>
           <cell r="H5" t="str">
-            <v>0.0025</v>
+            <v>0.0026</v>
           </cell>
         </row>
         <row r="6">
@@ -662,11 +625,8 @@
           <cell r="D6" t="str">
             <v>(42.6)</v>
           </cell>
-          <cell r="E6" t="str">
-            <v>(4.65)</v>
-          </cell>
           <cell r="F6" t="str">
-            <v>(2.88)</v>
+            <v>(2.89)</v>
           </cell>
           <cell r="G6" t="str">
             <v>(0.015)</v>
@@ -695,9 +655,6 @@
           <cell r="D83" t="str">
             <v/>
           </cell>
-          <cell r="E83" t="str">
-            <v/>
-          </cell>
           <cell r="F83" t="str">
             <v/>
           </cell>
@@ -708,7 +665,7 @@
             <v/>
           </cell>
           <cell r="I83" t="str">
-            <v>0.88***</v>
+            <v>0.88</v>
           </cell>
         </row>
         <row r="84">
@@ -722,9 +679,6 @@
             <v/>
           </cell>
           <cell r="D84" t="str">
-            <v/>
-          </cell>
-          <cell r="E84" t="str">
             <v/>
           </cell>
           <cell r="F84" t="str">
@@ -752,28 +706,25 @@
         </row>
         <row r="101">
           <cell r="B101" t="str">
-            <v>5921</v>
+            <v>5922</v>
           </cell>
           <cell r="C101" t="str">
-            <v>6036</v>
+            <v>6037</v>
           </cell>
           <cell r="D101" t="str">
-            <v>6036</v>
-          </cell>
-          <cell r="E101" t="str">
-            <v>3118</v>
+            <v>6037</v>
           </cell>
           <cell r="F101" t="str">
-            <v>2638</v>
+            <v>2639</v>
           </cell>
           <cell r="G101" t="str">
-            <v>6036</v>
+            <v>6037</v>
           </cell>
           <cell r="H101" t="str">
-            <v>5996</v>
+            <v>5997</v>
           </cell>
           <cell r="I101" t="str">
-            <v>5996</v>
+            <v>5997</v>
           </cell>
         </row>
       </sheetData>
@@ -798,13 +749,10 @@
             <v>0.049</v>
           </cell>
           <cell r="D5" t="str">
-            <v>-91.6*</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>7.84</v>
+            <v>-90.2</v>
           </cell>
           <cell r="F5" t="str">
-            <v>-2.99</v>
+            <v>-3.00</v>
           </cell>
           <cell r="G5" t="str">
             <v>-0.021</v>
@@ -821,10 +769,7 @@
             <v>(0.042)</v>
           </cell>
           <cell r="D6" t="str">
-            <v>(53.3)</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>(4.78)</v>
+            <v>(53.4)</v>
           </cell>
           <cell r="F6" t="str">
             <v>(3.14)</v>
@@ -856,9 +801,6 @@
           <cell r="D83" t="str">
             <v/>
           </cell>
-          <cell r="E83" t="str">
-            <v/>
-          </cell>
           <cell r="F83" t="str">
             <v/>
           </cell>
@@ -869,7 +811,7 @@
             <v/>
           </cell>
           <cell r="I83" t="str">
-            <v>0.89***</v>
+            <v>0.89</v>
           </cell>
         </row>
         <row r="84">
@@ -885,9 +827,6 @@
           <cell r="D84" t="str">
             <v/>
           </cell>
-          <cell r="E84" t="str">
-            <v/>
-          </cell>
           <cell r="F84" t="str">
             <v/>
           </cell>
@@ -903,7 +842,7 @@
         </row>
         <row r="95">
           <cell r="I95" t="str">
-            <v>-0.0081</v>
+            <v>-0.0080</v>
           </cell>
         </row>
         <row r="96">
@@ -920,9 +859,6 @@
           </cell>
           <cell r="D101" t="str">
             <v>5368</v>
-          </cell>
-          <cell r="E101" t="str">
-            <v>2786</v>
           </cell>
           <cell r="F101" t="str">
             <v>2334</v>
@@ -1240,37 +1176,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46C08B4-F7E1-44E4-85EC-7044A9D4DD25}">
-  <dimension ref="A2:I41"/>
+  <dimension ref="A2:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H40" sqref="A2:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="8.88671875" style="1"/>
+    <col min="2" max="8" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>2</v>
@@ -1278,18 +1213,15 @@
       <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="str">
         <f>[1]mechanism_pro_2!A2</f>
         <v/>
@@ -1302,13 +1234,12 @@
         <f>[1]mechanism_pro_2!C2</f>
         <v>(2)</v>
       </c>
-      <c r="D4" s="4" t="str">
+      <c r="D4" s="10" t="str">
         <f>[1]mechanism_pro_2!D2</f>
         <v>(3)</v>
       </c>
-      <c r="E4" s="4" t="str">
-        <f>[1]mechanism_pro_2!E2</f>
-        <v>(4)</v>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="F4" s="4" t="str">
         <f>[1]mechanism_pro_2!F2</f>
@@ -1322,50 +1253,42 @@
         <f>[1]mechanism_pro_2!H2</f>
         <v>(7)</v>
       </c>
-      <c r="I4" s="4" t="str">
-        <f>[1]mechanism_pro_2!I2</f>
-        <v>(8)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>[1]mechanism_pro_2!B5</f>
-        <v>-8.54***</v>
+        <v>-8.54</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>[1]mechanism_pro_2!C5</f>
-        <v>0.19***</v>
+        <v>0.19</v>
       </c>
       <c r="D6" s="1" t="str">
         <f>[1]mechanism_pro_2!D5</f>
-        <v>37.7</v>
+        <v>34.0</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f>[1]mechanism_pro_2!E5</f>
-        <v>15.5***</v>
+        <f>[1]mechanism_pro_2!F5</f>
+        <v>-8.52</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>[1]mechanism_pro_2!F5</f>
-        <v>-8.51***</v>
-      </c>
-      <c r="G6" s="1" t="str">
         <f>[1]mechanism_pro_2!G5</f>
         <v>-0.0068</v>
       </c>
+      <c r="G6" s="1" t="str">
+        <f>[1]mechanism_pro_2!H5</f>
+        <v>0.081</v>
+      </c>
       <c r="H6" s="1" t="str">
-        <f>[1]mechanism_pro_2!H5</f>
-        <v>0.081***</v>
-      </c>
-      <c r="I6" s="1" t="str">
         <f>[1]mechanism_pro_2!I77</f>
         <v>-0.017</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="str">
         <f>[1]mechanism_pro_2!B6</f>
         <v>(1.03)</v>
@@ -1376,45 +1299,41 @@
       </c>
       <c r="D7" s="1" t="str">
         <f>[1]mechanism_pro_2!D6</f>
-        <v>(51.0)</v>
+        <v>(51.2)</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f>[1]mechanism_pro_2!E6</f>
-        <v>(4.57)</v>
-      </c>
-      <c r="F7" s="1" t="str">
         <f>[1]mechanism_pro_2!F6</f>
         <v>(2.68)</v>
       </c>
-      <c r="G7" s="1" t="str">
+      <c r="F7" s="1" t="str">
         <f>[1]mechanism_pro_2!G6</f>
         <v>(0.018)</v>
       </c>
-      <c r="H7" s="1" t="str">
+      <c r="G7" s="1" t="str">
         <f>[1]mechanism_pro_2!H6</f>
         <v>(0.025)</v>
       </c>
-      <c r="I7" s="1" t="str">
+      <c r="H7" s="1" t="str">
         <f>[1]mechanism_pro_2!I78</f>
         <v>(0.028)</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="1" t="str">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="str">
         <f>[1]mechanism_pro_2!I95</f>
         <v>-0.0042</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I9" s="1" t="str">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="1" t="str">
         <f>[1]mechanism_pro_2!I96</f>
         <v>(0.030)</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1431,27 +1350,23 @@
         <v/>
       </c>
       <c r="E10" s="1" t="str">
-        <f>[1]mechanism_pro_2!E83</f>
+        <f>[1]mechanism_pro_2!F83</f>
         <v/>
       </c>
       <c r="F10" s="1" t="str">
-        <f>[1]mechanism_pro_2!F83</f>
+        <f>[1]mechanism_pro_2!G83</f>
         <v/>
       </c>
       <c r="G10" s="1" t="str">
-        <f>[1]mechanism_pro_2!G83</f>
+        <f>[1]mechanism_pro_2!H83</f>
         <v/>
       </c>
       <c r="H10" s="1" t="str">
-        <f>[1]mechanism_pro_2!H83</f>
-        <v/>
-      </c>
-      <c r="I10" s="1" t="str">
         <f>[1]mechanism_pro_2!I83</f>
-        <v>0.88***</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>[1]mechanism_pro_2!A84</f>
         <v/>
@@ -1469,27 +1384,23 @@
         <v/>
       </c>
       <c r="E11" s="1" t="str">
-        <f>[1]mechanism_pro_2!E84</f>
+        <f>[1]mechanism_pro_2!F84</f>
         <v/>
       </c>
       <c r="F11" s="1" t="str">
-        <f>[1]mechanism_pro_2!F84</f>
+        <f>[1]mechanism_pro_2!G84</f>
         <v/>
       </c>
       <c r="G11" s="1" t="str">
-        <f>[1]mechanism_pro_2!G84</f>
+        <f>[1]mechanism_pro_2!H84</f>
         <v/>
       </c>
       <c r="H11" s="1" t="str">
-        <f>[1]mechanism_pro_2!H84</f>
-        <v/>
-      </c>
-      <c r="I11" s="1" t="str">
         <f>[1]mechanism_pro_2!I84</f>
         <v>(0.017)</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1506,51 +1417,46 @@
         <v>5085</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f>[1]mechanism_pro_2!E101</f>
-        <v>2719</v>
-      </c>
-      <c r="F12" s="3" t="str">
         <f>[1]mechanism_pro_2!F101</f>
         <v>2490</v>
       </c>
-      <c r="G12" s="3" t="str">
+      <c r="F12" s="3" t="str">
         <f>[1]mechanism_pro_2!G101</f>
         <v>5085</v>
       </c>
-      <c r="H12" s="3" t="str">
+      <c r="G12" s="3" t="str">
         <f>[1]mechanism_pro_2!H101</f>
         <v>5062</v>
       </c>
-      <c r="I12" s="3" t="str">
+      <c r="H12" s="3" t="str">
         <f>[1]mechanism_pro_2!I101</f>
         <v>5062</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>12</v>
@@ -1564,48 +1470,41 @@
       <c r="H14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="str">
         <f>[2]mechanism_pro_3!B5</f>
-        <v>-3.01***</v>
+        <v>-2.97</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>[2]mechanism_pro_3!C5</f>
-        <v>0.17***</v>
+        <v>0.17</v>
       </c>
       <c r="D15" s="1" t="str">
         <f>[2]mechanism_pro_3!D5</f>
-        <v>-68.8</v>
+        <v>-72.6</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f>[2]mechanism_pro_3!E5</f>
-        <v>20.1***</v>
+        <f>[2]mechanism_pro_3!F5</f>
+        <v>-1.45</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>[2]mechanism_pro_3!F5</f>
-        <v>-1.59</v>
-      </c>
-      <c r="G15" s="1" t="str">
         <f>[2]mechanism_pro_3!G5</f>
         <v>-0.021</v>
       </c>
-      <c r="H15" s="1" t="str">
+      <c r="G15" s="1" t="str">
         <f>[2]mechanism_pro_3!H5</f>
         <v>-0.0049</v>
       </c>
-      <c r="I15" s="1" t="str">
+      <c r="H15" s="1" t="str">
         <f>[2]mechanism_pro_3!I77</f>
         <v>-0.012</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="str">
         <f>[2]mechanism_pro_3!B6</f>
         <v>(1.13)</v>
@@ -1616,45 +1515,41 @@
       </c>
       <c r="D16" s="1" t="str">
         <f>[2]mechanism_pro_3!D6</f>
-        <v>(46.6)</v>
+        <v>(46.5)</v>
       </c>
       <c r="E16" s="1" t="str">
-        <f>[2]mechanism_pro_3!E6</f>
-        <v>(5.51)</v>
+        <f>[2]mechanism_pro_3!F6</f>
+        <v>(3.21)</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>[2]mechanism_pro_3!F6</f>
-        <v>(3.22)</v>
-      </c>
-      <c r="G16" s="1" t="str">
         <f>[2]mechanism_pro_3!G6</f>
         <v>(0.020)</v>
       </c>
-      <c r="H16" s="1" t="str">
+      <c r="G16" s="1" t="str">
         <f>[2]mechanism_pro_3!H6</f>
         <v>(0.026)</v>
       </c>
-      <c r="I16" s="1" t="str">
+      <c r="H16" s="1" t="str">
         <f>[2]mechanism_pro_3!I78</f>
         <v>(0.028)</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="1" t="str">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="str">
         <f>[2]mechanism_pro_3!I95</f>
-        <v>0.0063</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I18" s="1" t="str">
+        <v>0.0060</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H18" s="1" t="str">
         <f>[2]mechanism_pro_3!I96</f>
         <v>(0.028)</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1671,27 +1566,23 @@
         <v/>
       </c>
       <c r="E19" s="1" t="str">
-        <f>[2]mechanism_pro_3!E83</f>
+        <f>[2]mechanism_pro_3!F83</f>
         <v/>
       </c>
       <c r="F19" s="1" t="str">
-        <f>[2]mechanism_pro_3!F83</f>
+        <f>[2]mechanism_pro_3!G83</f>
         <v/>
       </c>
       <c r="G19" s="1" t="str">
-        <f>[2]mechanism_pro_3!G83</f>
+        <f>[2]mechanism_pro_3!H83</f>
         <v/>
       </c>
       <c r="H19" s="1" t="str">
-        <f>[2]mechanism_pro_3!H83</f>
-        <v/>
-      </c>
-      <c r="I19" s="1" t="str">
         <f>[2]mechanism_pro_3!I83</f>
-        <v>0.88***</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>[2]mechanism_pro_3!A84</f>
         <v/>
@@ -1709,88 +1600,79 @@
         <v/>
       </c>
       <c r="E20" s="1" t="str">
-        <f>[2]mechanism_pro_3!E84</f>
+        <f>[2]mechanism_pro_3!F84</f>
         <v/>
       </c>
       <c r="F20" s="1" t="str">
-        <f>[2]mechanism_pro_3!F84</f>
+        <f>[2]mechanism_pro_3!G84</f>
         <v/>
       </c>
       <c r="G20" s="1" t="str">
-        <f>[2]mechanism_pro_3!G84</f>
+        <f>[2]mechanism_pro_3!H84</f>
         <v/>
       </c>
       <c r="H20" s="1" t="str">
-        <f>[2]mechanism_pro_3!H84</f>
-        <v/>
-      </c>
-      <c r="I20" s="1" t="str">
         <f>[2]mechanism_pro_3!I84</f>
         <v>(0.017)</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="3" t="str">
         <f>[2]mechanism_pro_3!B101</f>
-        <v>4656</v>
+        <v>4655</v>
       </c>
       <c r="C21" s="3" t="str">
         <f>[2]mechanism_pro_3!C101</f>
-        <v>4758</v>
+        <v>4757</v>
       </c>
       <c r="D21" s="3" t="str">
         <f>[2]mechanism_pro_3!D101</f>
-        <v>4758</v>
+        <v>4757</v>
       </c>
       <c r="E21" s="3" t="str">
-        <f>[2]mechanism_pro_3!E101</f>
-        <v>2409</v>
+        <f>[2]mechanism_pro_3!F101</f>
+        <v>2073</v>
       </c>
       <c r="F21" s="3" t="str">
-        <f>[2]mechanism_pro_3!F101</f>
-        <v>2075</v>
+        <f>[2]mechanism_pro_3!G101</f>
+        <v>4757</v>
       </c>
       <c r="G21" s="3" t="str">
-        <f>[2]mechanism_pro_3!G101</f>
-        <v>4758</v>
+        <f>[2]mechanism_pro_3!H101</f>
+        <v>4733</v>
       </c>
       <c r="H21" s="3" t="str">
-        <f>[2]mechanism_pro_3!H101</f>
-        <v>4734</v>
-      </c>
-      <c r="I21" s="3" t="str">
         <f>[2]mechanism_pro_3!I101</f>
-        <v>4734</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4733</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>12</v>
@@ -1804,48 +1686,41 @@
       <c r="H23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="str">
         <f>[3]mechanism_pro_4!B5</f>
-        <v>-2.38**</v>
+        <v>-2.40</v>
       </c>
       <c r="C24" s="1" t="str">
         <f>[3]mechanism_pro_4!C5</f>
-        <v>0.13***</v>
+        <v>0.13</v>
       </c>
       <c r="D24" s="1" t="str">
         <f>[3]mechanism_pro_4!D5</f>
-        <v>-54.2</v>
+        <v>-53.7</v>
       </c>
       <c r="E24" s="1" t="str">
-        <f>[3]mechanism_pro_4!E5</f>
-        <v>16.5***</v>
+        <f>[3]mechanism_pro_4!F5</f>
+        <v>0.98</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>[3]mechanism_pro_4!F5</f>
-        <v>1.02</v>
-      </c>
-      <c r="G24" s="1" t="str">
         <f>[3]mechanism_pro_4!G5</f>
         <v>-0.0077</v>
       </c>
+      <c r="G24" s="1" t="str">
+        <f>[3]mechanism_pro_4!H5</f>
+        <v>0.0026</v>
+      </c>
       <c r="H24" s="1" t="str">
-        <f>[3]mechanism_pro_4!H5</f>
-        <v>0.0025</v>
-      </c>
-      <c r="I24" s="1" t="str">
         <f>[3]mechanism_pro_4!I77</f>
         <v>-0.013</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="str">
         <f>[3]mechanism_pro_4!B6</f>
         <v>(0.97)</v>
@@ -1859,42 +1734,38 @@
         <v>(42.6)</v>
       </c>
       <c r="E25" s="1" t="str">
-        <f>[3]mechanism_pro_4!E6</f>
-        <v>(4.65)</v>
+        <f>[3]mechanism_pro_4!F6</f>
+        <v>(2.89)</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>[3]mechanism_pro_4!F6</f>
-        <v>(2.88)</v>
-      </c>
-      <c r="G25" s="1" t="str">
         <f>[3]mechanism_pro_4!G6</f>
         <v>(0.015)</v>
       </c>
-      <c r="H25" s="1" t="str">
+      <c r="G25" s="1" t="str">
         <f>[3]mechanism_pro_4!H6</f>
         <v>(0.020)</v>
       </c>
-      <c r="I25" s="1" t="str">
+      <c r="H25" s="1" t="str">
         <f>[3]mechanism_pro_4!I78</f>
         <v>(0.019)</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="I26" s="1" t="str">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1" t="str">
         <f>[3]mechanism_pro_4!I95</f>
         <v>0.013</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I27" s="1" t="str">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H27" s="1" t="str">
         <f>[3]mechanism_pro_4!I96</f>
         <v>(0.020)</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1911,27 +1782,23 @@
         <v/>
       </c>
       <c r="E28" s="1" t="str">
-        <f>[3]mechanism_pro_4!E83</f>
+        <f>[3]mechanism_pro_4!F83</f>
         <v/>
       </c>
       <c r="F28" s="1" t="str">
-        <f>[3]mechanism_pro_4!F83</f>
+        <f>[3]mechanism_pro_4!G83</f>
         <v/>
       </c>
       <c r="G28" s="1" t="str">
-        <f>[3]mechanism_pro_4!G83</f>
+        <f>[3]mechanism_pro_4!H83</f>
         <v/>
       </c>
       <c r="H28" s="1" t="str">
-        <f>[3]mechanism_pro_4!H83</f>
-        <v/>
-      </c>
-      <c r="I28" s="1" t="str">
         <f>[3]mechanism_pro_4!I83</f>
-        <v>0.88***</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>[3]mechanism_pro_4!A84</f>
         <v/>
@@ -1949,88 +1816,79 @@
         <v/>
       </c>
       <c r="E29" s="1" t="str">
-        <f>[3]mechanism_pro_4!E84</f>
+        <f>[3]mechanism_pro_4!F84</f>
         <v/>
       </c>
       <c r="F29" s="1" t="str">
-        <f>[3]mechanism_pro_4!F84</f>
+        <f>[3]mechanism_pro_4!G84</f>
         <v/>
       </c>
       <c r="G29" s="1" t="str">
-        <f>[3]mechanism_pro_4!G84</f>
+        <f>[3]mechanism_pro_4!H84</f>
         <v/>
       </c>
       <c r="H29" s="1" t="str">
-        <f>[3]mechanism_pro_4!H84</f>
-        <v/>
-      </c>
-      <c r="I29" s="1" t="str">
         <f>[3]mechanism_pro_4!I84</f>
         <v>(0.017)</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="3" t="str">
         <f>[3]mechanism_pro_4!B101</f>
-        <v>5921</v>
+        <v>5922</v>
       </c>
       <c r="C30" s="3" t="str">
         <f>[3]mechanism_pro_4!C101</f>
-        <v>6036</v>
+        <v>6037</v>
       </c>
       <c r="D30" s="3" t="str">
         <f>[3]mechanism_pro_4!D101</f>
-        <v>6036</v>
+        <v>6037</v>
       </c>
       <c r="E30" s="3" t="str">
-        <f>[3]mechanism_pro_4!E101</f>
-        <v>3118</v>
+        <f>[3]mechanism_pro_4!F101</f>
+        <v>2639</v>
       </c>
       <c r="F30" s="3" t="str">
-        <f>[3]mechanism_pro_4!F101</f>
-        <v>2638</v>
+        <f>[3]mechanism_pro_4!G101</f>
+        <v>6037</v>
       </c>
       <c r="G30" s="3" t="str">
-        <f>[3]mechanism_pro_4!G101</f>
-        <v>6036</v>
+        <f>[3]mechanism_pro_4!H101</f>
+        <v>5997</v>
       </c>
       <c r="H30" s="3" t="str">
-        <f>[3]mechanism_pro_4!H101</f>
-        <v>5996</v>
-      </c>
-      <c r="I30" s="3" t="str">
         <f>[3]mechanism_pro_4!I101</f>
-        <v>5996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>5997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>12</v>
@@ -2044,13 +1902,10 @@
       <c r="H32" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I32" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="1" t="str">
         <f>[4]mechanism_pro_5!B5</f>
@@ -2062,30 +1917,26 @@
       </c>
       <c r="D33" s="1" t="str">
         <f>[4]mechanism_pro_5!D5</f>
-        <v>-91.6*</v>
+        <v>-90.2</v>
       </c>
       <c r="E33" s="1" t="str">
-        <f>[4]mechanism_pro_5!E5</f>
-        <v>7.84</v>
+        <f>[4]mechanism_pro_5!F5</f>
+        <v>-3.00</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>[4]mechanism_pro_5!F5</f>
-        <v>-2.99</v>
-      </c>
-      <c r="G33" s="1" t="str">
         <f>[4]mechanism_pro_5!G5</f>
         <v>-0.021</v>
       </c>
-      <c r="H33" s="1" t="str">
+      <c r="G33" s="1" t="str">
         <f>[4]mechanism_pro_5!H5</f>
         <v>-0.015</v>
       </c>
-      <c r="I33" s="1" t="str">
+      <c r="H33" s="1" t="str">
         <f>[4]mechanism_pro_5!I77</f>
         <v>-0.0049</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="str">
         <f>[4]mechanism_pro_5!B6</f>
         <v>(0.94)</v>
@@ -2096,45 +1947,41 @@
       </c>
       <c r="D34" s="1" t="str">
         <f>[4]mechanism_pro_5!D6</f>
-        <v>(53.3)</v>
+        <v>(53.4)</v>
       </c>
       <c r="E34" s="1" t="str">
-        <f>[4]mechanism_pro_5!E6</f>
-        <v>(4.78)</v>
-      </c>
-      <c r="F34" s="1" t="str">
         <f>[4]mechanism_pro_5!F6</f>
         <v>(3.14)</v>
       </c>
-      <c r="G34" s="1" t="str">
+      <c r="F34" s="1" t="str">
         <f>[4]mechanism_pro_5!G6</f>
         <v>(0.017)</v>
       </c>
-      <c r="H34" s="1" t="str">
+      <c r="G34" s="1" t="str">
         <f>[4]mechanism_pro_5!H6</f>
         <v>(0.023)</v>
       </c>
-      <c r="I34" s="1" t="str">
+      <c r="H34" s="1" t="str">
         <f>[4]mechanism_pro_5!I78</f>
         <v>(0.025)</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="I35" s="1" t="str">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1" t="str">
         <f>[4]mechanism_pro_5!I95</f>
-        <v>-0.0081</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I36" s="1" t="str">
+        <v>-0.0080</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="1" t="str">
         <f>[4]mechanism_pro_5!I96</f>
         <v>(0.026)</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -2151,27 +1998,23 @@
         <v/>
       </c>
       <c r="E37" s="1" t="str">
-        <f>[4]mechanism_pro_5!E83</f>
+        <f>[4]mechanism_pro_5!F83</f>
         <v/>
       </c>
       <c r="F37" s="1" t="str">
-        <f>[4]mechanism_pro_5!F83</f>
+        <f>[4]mechanism_pro_5!G83</f>
         <v/>
       </c>
       <c r="G37" s="1" t="str">
-        <f>[4]mechanism_pro_5!G83</f>
+        <f>[4]mechanism_pro_5!H83</f>
         <v/>
       </c>
       <c r="H37" s="1" t="str">
-        <f>[4]mechanism_pro_5!H83</f>
-        <v/>
-      </c>
-      <c r="I37" s="1" t="str">
         <f>[4]mechanism_pro_5!I83</f>
-        <v>0.89***</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>[4]mechanism_pro_5!A84</f>
         <v/>
@@ -2189,27 +2032,23 @@
         <v/>
       </c>
       <c r="E38" s="1" t="str">
-        <f>[4]mechanism_pro_5!E84</f>
+        <f>[4]mechanism_pro_5!F84</f>
         <v/>
       </c>
       <c r="F38" s="1" t="str">
-        <f>[4]mechanism_pro_5!F84</f>
+        <f>[4]mechanism_pro_5!G84</f>
         <v/>
       </c>
       <c r="G38" s="1" t="str">
-        <f>[4]mechanism_pro_5!G84</f>
+        <f>[4]mechanism_pro_5!H84</f>
         <v/>
       </c>
       <c r="H38" s="1" t="str">
-        <f>[4]mechanism_pro_5!H84</f>
-        <v/>
-      </c>
-      <c r="I38" s="1" t="str">
         <f>[4]mechanism_pro_5!I84</f>
         <v>(0.017)</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
@@ -2226,27 +2065,23 @@
         <v>5368</v>
       </c>
       <c r="E39" s="3" t="str">
-        <f>[4]mechanism_pro_5!E101</f>
-        <v>2786</v>
-      </c>
-      <c r="F39" s="3" t="str">
         <f>[4]mechanism_pro_5!F101</f>
         <v>2334</v>
       </c>
-      <c r="G39" s="3" t="str">
+      <c r="F39" s="3" t="str">
         <f>[4]mechanism_pro_5!G101</f>
         <v>5368</v>
       </c>
-      <c r="H39" s="3" t="str">
+      <c r="G39" s="3" t="str">
         <f>[4]mechanism_pro_5!H101</f>
         <v>5346</v>
       </c>
-      <c r="I39" s="3" t="str">
+      <c r="H39" s="3" t="str">
         <f>[4]mechanism_pro_5!I101</f>
         <v>5346</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="str">
         <f>[1]mechanism_pro_2!A103</f>
         <v>Control Mean</v>
@@ -2261,37 +2096,33 @@
       </c>
       <c r="D40" s="8" t="str">
         <f>[1]mechanism_pro_2!D103</f>
-        <v>829.7</v>
+        <v>830.5</v>
       </c>
       <c r="E40" s="8" t="str">
-        <f>[1]mechanism_pro_2!E103</f>
-        <v>81.7</v>
-      </c>
-      <c r="F40" s="8" t="str">
         <f>[1]mechanism_pro_2!F103</f>
         <v>92.7</v>
       </c>
-      <c r="G40" s="8" t="str">
+      <c r="F40" s="8" t="str">
         <f>[1]mechanism_pro_2!G103</f>
         <v>0.75</v>
       </c>
-      <c r="H40" s="8" t="str">
+      <c r="G40" s="8" t="str">
         <f>[1]mechanism_pro_2!H103</f>
         <v>0.73</v>
       </c>
-      <c r="I40" s="8" t="str">
+      <c r="H40" s="8" t="str">
         <f>[1]mechanism_pro_2!I103</f>
         <v>0.73</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>